<commit_message>
PROS-6212 BIVN template update for Jul & Aug 2018 with correct category/brand
</commit_message>
<xml_diff>
--- a/Projects/BIMY/Data/Template_Aug_2018.xlsx
+++ b/Projects/BIMY/Data/Template_Aug_2018.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Deeksha\Documents\final templates\Brand block recal\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Deeksha\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{478CC9F9-195A-4BE3-AA1B-654D0E8DFE67}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{C6419EBE-95E2-49BF-96D2-7A8217B28D7E}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6960" firstSheet="4" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6090" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="KPIs" sheetId="7" r:id="rId1"/>
@@ -704,18 +704,12 @@
     <t>4048846005328</t>
   </si>
   <si>
-    <t>DULCOLAX TAB 200S (BLISTER PACK) - NEW</t>
-  </si>
-  <si>
     <t>9556991220299</t>
   </si>
   <si>
     <t>Dulcolax</t>
   </si>
   <si>
-    <t>DULCOLAX TABLETS 30's</t>
-  </si>
-  <si>
     <t>9556991220282</t>
   </si>
   <si>
@@ -834,6 +828,12 @@
   </si>
   <si>
     <t>MY_Secondary_0818</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DULCOLAX TAB 200S (BLISTER PACK) </t>
+  </si>
+  <si>
+    <t>DULCOLAX TAB 30S (BLISTER PACK)</t>
   </si>
 </sst>
 </file>
@@ -1018,7 +1018,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="20">
+  <fills count="19">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1124,12 +1124,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
-        <bgColor rgb="FFF2F2F2"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor rgb="FFDAE3F3"/>
       </patternFill>
     </fill>
@@ -1408,7 +1402,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="108">
+  <cellXfs count="105">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="7" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1677,16 +1671,10 @@
     <xf numFmtId="0" fontId="9" fillId="17" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="9" fillId="16" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1695,23 +1683,19 @@
     <xf numFmtId="0" fontId="6" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="16" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2360,8 +2344,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2450,13 +2434,13 @@
         <v>5</v>
       </c>
       <c r="B5" s="53" t="s">
+        <v>92</v>
+      </c>
+      <c r="C5" s="54" t="s">
         <v>50</v>
       </c>
-      <c r="C5" s="54" t="s">
+      <c r="D5" s="55" t="s">
         <v>51</v>
-      </c>
-      <c r="D5" s="55" t="s">
-        <v>52</v>
       </c>
       <c r="E5" s="56" t="s">
         <v>40</v>
@@ -2470,13 +2454,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="53" t="s">
-        <v>53</v>
+        <v>93</v>
       </c>
       <c r="C6" s="54" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D6" s="55" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E6" s="56" t="s">
         <v>40</v>
@@ -2490,13 +2474,13 @@
         <v>5</v>
       </c>
       <c r="B7" s="53" t="s">
+        <v>53</v>
+      </c>
+      <c r="C7" s="54" t="s">
+        <v>54</v>
+      </c>
+      <c r="D7" s="55" t="s">
         <v>55</v>
-      </c>
-      <c r="C7" s="54" t="s">
-        <v>56</v>
-      </c>
-      <c r="D7" s="55" t="s">
-        <v>57</v>
       </c>
       <c r="E7" s="56" t="s">
         <v>41</v>
@@ -2510,13 +2494,13 @@
         <v>5</v>
       </c>
       <c r="B8" s="53" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C8" s="54">
         <v>7610939003137</v>
       </c>
       <c r="D8" s="55" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E8" s="56" t="s">
         <v>41</v>
@@ -2530,13 +2514,13 @@
         <v>5</v>
       </c>
       <c r="B9" s="53" t="s">
+        <v>57</v>
+      </c>
+      <c r="C9" s="54" t="s">
+        <v>58</v>
+      </c>
+      <c r="D9" s="55" t="s">
         <v>59</v>
-      </c>
-      <c r="C9" s="54" t="s">
-        <v>60</v>
-      </c>
-      <c r="D9" s="55" t="s">
-        <v>61</v>
       </c>
       <c r="E9" s="56" t="s">
         <v>41</v>
@@ -2550,13 +2534,13 @@
         <v>5</v>
       </c>
       <c r="B10" s="53" t="s">
+        <v>60</v>
+      </c>
+      <c r="C10" s="54" t="s">
+        <v>61</v>
+      </c>
+      <c r="D10" s="55" t="s">
         <v>62</v>
-      </c>
-      <c r="C10" s="54" t="s">
-        <v>63</v>
-      </c>
-      <c r="D10" s="55" t="s">
-        <v>64</v>
       </c>
       <c r="E10" s="56" t="s">
         <v>39</v>
@@ -2570,13 +2554,13 @@
         <v>5</v>
       </c>
       <c r="B11" s="53" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C11" s="57">
         <v>9556499172861</v>
       </c>
       <c r="D11" s="55" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E11" s="56" t="s">
         <v>40</v>
@@ -2590,13 +2574,13 @@
         <v>5</v>
       </c>
       <c r="B12" s="53" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C12" s="57">
         <v>9556499331442</v>
       </c>
       <c r="D12" s="55" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E12" s="56" t="s">
         <v>40</v>
@@ -2610,10 +2594,10 @@
         <v>5</v>
       </c>
       <c r="B13" s="53" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C13" s="57" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D13" s="55" t="s">
         <v>42</v>
@@ -2630,10 +2614,10 @@
         <v>5</v>
       </c>
       <c r="B14" s="53" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C14" s="57" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D14" s="55" t="s">
         <v>42</v>
@@ -2650,13 +2634,13 @@
         <v>5</v>
       </c>
       <c r="B15" s="53" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C15" s="57">
         <v>3582910052104</v>
       </c>
       <c r="D15" s="55" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E15" s="56" t="s">
         <v>43</v>
@@ -2670,13 +2654,13 @@
         <v>5</v>
       </c>
       <c r="B16" s="53" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C16" s="57">
         <v>3582910009405</v>
       </c>
       <c r="D16" s="55" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E16" s="56" t="s">
         <v>12</v>
@@ -2690,13 +2674,13 @@
         <v>5</v>
       </c>
       <c r="B17" s="53" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C17" s="57">
         <v>3582910010296</v>
       </c>
       <c r="D17" s="55" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E17" s="56" t="s">
         <v>12</v>
@@ -2736,10 +2720,10 @@
       <c r="C1" s="10"/>
       <c r="D1" s="10"/>
       <c r="E1" s="10"/>
-      <c r="F1" s="96" t="s">
+      <c r="F1" s="102" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="97"/>
+      <c r="G1" s="103"/>
     </row>
     <row r="2" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
@@ -2995,10 +2979,10 @@
       <c r="D3" s="64" t="s">
         <v>48</v>
       </c>
-      <c r="E3" s="98" t="s">
+      <c r="E3" s="96" t="s">
         <v>49</v>
       </c>
-      <c r="F3" s="99">
+      <c r="F3" s="97">
         <v>1</v>
       </c>
     </row>
@@ -3007,18 +2991,18 @@
         <v>3</v>
       </c>
       <c r="B4" s="87" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C4" s="52" t="s">
         <v>12</v>
       </c>
       <c r="D4" s="64" t="s">
-        <v>90</v>
-      </c>
-      <c r="E4" s="100" t="s">
-        <v>86</v>
-      </c>
-      <c r="F4" s="99">
+        <v>88</v>
+      </c>
+      <c r="E4" s="98" t="s">
+        <v>84</v>
+      </c>
+      <c r="F4" s="97">
         <v>1</v>
       </c>
     </row>
@@ -3027,16 +3011,16 @@
         <v>3</v>
       </c>
       <c r="B5" s="65" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C5" s="63" t="s">
         <v>41</v>
       </c>
       <c r="D5" s="64" t="s">
-        <v>88</v>
-      </c>
-      <c r="E5" s="100" t="s">
-        <v>91</v>
+        <v>86</v>
+      </c>
+      <c r="E5" s="98" t="s">
+        <v>89</v>
       </c>
       <c r="F5" s="66">
         <v>1</v>
@@ -3053,10 +3037,10 @@
         <v>43</v>
       </c>
       <c r="D6" s="64" t="s">
-        <v>89</v>
-      </c>
-      <c r="E6" s="100" t="s">
         <v>87</v>
+      </c>
+      <c r="E6" s="98" t="s">
+        <v>85</v>
       </c>
       <c r="F6" s="66">
         <v>1</v>
@@ -3228,7 +3212,7 @@
   <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -3277,13 +3261,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="73" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C3" s="74" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D3" s="75" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E3" s="76" t="s">
         <v>12</v>
@@ -3297,13 +3281,13 @@
         <v>1</v>
       </c>
       <c r="B4" s="77" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C4" s="78" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D4" s="71" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E4" s="72" t="s">
         <v>41</v>
@@ -3317,10 +3301,10 @@
         <v>1</v>
       </c>
       <c r="B5" s="79" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C5" s="78" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D5" s="71" t="s">
         <v>42</v>
@@ -3337,15 +3321,15 @@
         <v>4</v>
       </c>
       <c r="B6" s="80" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C6" s="81" t="s">
-        <v>85</v>
-      </c>
-      <c r="D6" s="102" t="s">
-        <v>57</v>
-      </c>
-      <c r="E6" s="102" t="s">
+        <v>83</v>
+      </c>
+      <c r="D6" s="81" t="s">
+        <v>59</v>
+      </c>
+      <c r="E6" s="104" t="s">
         <v>41</v>
       </c>
       <c r="F6" s="82">
@@ -3353,22 +3337,22 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="101" t="s">
+      <c r="A7" s="99" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="103" t="s">
-        <v>92</v>
+      <c r="B7" s="80" t="s">
+        <v>90</v>
       </c>
       <c r="C7" s="81" t="s">
-        <v>93</v>
-      </c>
-      <c r="D7" s="102" t="s">
-        <v>57</v>
-      </c>
-      <c r="E7" s="102" t="s">
+        <v>91</v>
+      </c>
+      <c r="D7" s="81" t="s">
+        <v>55</v>
+      </c>
+      <c r="E7" s="104" t="s">
         <v>41</v>
       </c>
-      <c r="F7" s="104">
+      <c r="F7" s="82">
         <v>1</v>
       </c>
     </row>
@@ -3438,9 +3422,12 @@
       <c r="F26" s="3"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D6" r:id="rId1" tooltip="Essentiale" display="https://services.traxretail.com/trax-one/bimy/products-and-brands/brand/34" xr:uid="{2900A8DC-6C77-45D9-8DE1-C73295E63FE7}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -3448,8 +3435,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3518,13 +3505,13 @@
         <v>2</v>
       </c>
       <c r="B4" s="88" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C4" s="90">
         <v>3582910009405</v>
       </c>
       <c r="D4" s="87" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E4" s="87" t="s">
         <v>12</v>
@@ -3538,13 +3525,13 @@
         <v>2</v>
       </c>
       <c r="B5" s="88" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C5" s="90">
         <v>3582910010296</v>
       </c>
       <c r="D5" s="87" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E5" s="87" t="s">
         <v>12</v>
@@ -3558,7 +3545,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="88" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C6" s="90">
         <v>8993237276046</v>
@@ -3578,7 +3565,7 @@
         <v>2</v>
       </c>
       <c r="B7" s="88" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C7" s="90">
         <v>7891058013271</v>
@@ -3598,13 +3585,13 @@
         <v>2</v>
       </c>
       <c r="B8" s="88" t="s">
+        <v>53</v>
+      </c>
+      <c r="C8" s="89" t="s">
+        <v>54</v>
+      </c>
+      <c r="D8" s="87" t="s">
         <v>55</v>
-      </c>
-      <c r="C8" s="89" t="s">
-        <v>56</v>
-      </c>
-      <c r="D8" s="87" t="s">
-        <v>57</v>
       </c>
       <c r="E8" s="87" t="s">
         <v>41</v>
@@ -3618,13 +3605,13 @@
         <v>2</v>
       </c>
       <c r="B9" s="88" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C9" s="89">
         <v>7610939003137</v>
       </c>
       <c r="D9" s="87" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E9" s="87" t="s">
         <v>41</v>
@@ -3638,38 +3625,38 @@
         <v>36</v>
       </c>
       <c r="B10" s="92" t="s">
+        <v>57</v>
+      </c>
+      <c r="C10" s="93" t="s">
+        <v>58</v>
+      </c>
+      <c r="D10" s="94" t="s">
         <v>59</v>
       </c>
-      <c r="C10" s="93" t="s">
-        <v>60</v>
-      </c>
-      <c r="D10" s="94" t="s">
-        <v>61</v>
-      </c>
       <c r="E10" s="94" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F10" s="95">
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A11" s="105" t="s">
+      <c r="A11" s="100" t="s">
         <v>36</v>
       </c>
-      <c r="B11" s="106" t="s">
+      <c r="B11" s="92" t="s">
+        <v>53</v>
+      </c>
+      <c r="C11" s="93" t="s">
+        <v>54</v>
+      </c>
+      <c r="D11" s="94" t="s">
         <v>55</v>
       </c>
-      <c r="C11" s="93" t="s">
-        <v>56</v>
-      </c>
-      <c r="D11" s="106" t="s">
-        <v>57</v>
-      </c>
-      <c r="E11" s="106" t="s">
+      <c r="E11" s="94" t="s">
         <v>41</v>
       </c>
-      <c r="F11" s="107">
+      <c r="F11" s="101">
         <v>1</v>
       </c>
     </row>

</xml_diff>